<commit_message>
transfer files from archive version of the local repo
</commit_message>
<xml_diff>
--- a/ClientInformationRequests/ProjTracking/AD_ProjectTracking.xlsx
+++ b/ClientInformationRequests/ProjTracking/AD_ProjectTracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Common\Amazon Web Services Project\APPDEV Team\AutomationDesign\ClientInformationRequests\ProjRepo\ClientInformationRequests\ClientInformationRequests\ProjTracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://massgov-my.sharepoint.com/personal/andrew_walker_mass_gov/Documents/HomeDrive/Projects/repos/ClientInformationRequests/ClientInformationRequests/ProjTracking/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5274DDA-4E04-46FF-9900-1BA88BD91978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="17100" windowHeight="8510" tabRatio="580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5600" yWindow="1210" windowWidth="18770" windowHeight="9860" tabRatio="580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dev't Tracking" sheetId="1" r:id="rId1"/>
@@ -672,11 +672,11 @@
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <f ca="1">NOW()</f>
-        <v>44886.590117708336</v>
+        <v>45547.498554513892</v>
       </c>
       <c r="B2" s="4">
         <f ca="1">NOW()</f>
-        <v>44886.590117708336</v>
+        <v>45547.498554513892</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
@@ -930,7 +930,7 @@
     <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="C29" s="4">
         <f ca="1">NOW()</f>
-        <v>44886.590117708336</v>
+        <v>45547.498554513892</v>
       </c>
     </row>
     <row r="30" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -1897,15 +1897,15 @@
       </c>
       <c r="C71" s="4">
         <f ca="1">NOW()</f>
-        <v>44886.590117708336</v>
+        <v>45547.498554513892</v>
       </c>
       <c r="D71">
         <f t="shared" ca="1" si="60"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E71">
         <f t="shared" ca="1" si="61"/>
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="G71" t="s">
         <v>57</v>
@@ -2037,15 +2037,15 @@
       </c>
       <c r="C77" s="4">
         <f ca="1">NOW()</f>
-        <v>44886.590117708336</v>
+        <v>45547.498554513892</v>
       </c>
       <c r="D77">
         <f t="shared" ref="D77" ca="1" si="70">HOUR(C77-B77)</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E77">
         <f t="shared" ref="E77" ca="1" si="71">MINUTE(C77-B77)</f>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="G77" t="s">
         <v>43</v>
@@ -3124,7 +3124,7 @@
     <row r="126" spans="1:21" x14ac:dyDescent="0.35">
       <c r="C126" s="4">
         <f ca="1">NOW()</f>
-        <v>44886.590117708336</v>
+        <v>45547.498554513892</v>
       </c>
     </row>
     <row r="127" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -3175,7 +3175,7 @@
     <row r="129" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C129" s="4">
         <f ca="1">NOW()</f>
-        <v>44886.590117708336</v>
+        <v>45547.498554513892</v>
       </c>
     </row>
   </sheetData>

</xml_diff>